<commit_message>
weekly market data for dec 12
</commit_message>
<xml_diff>
--- a/BiceExpanded EXTRAS/EVE MARKET DATA/Union Modern.xlsx
+++ b/BiceExpanded EXTRAS/EVE MARKET DATA/Union Modern.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chimera\Documents\Paradox Interactive\Hearts of Iron IV\mod\BlackICE-ExpandedLocal\BiceExpanded EXTRAS\EVE MARKET DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James Rankin\Documents\Paradox Interactive\Hearts of Iron IV\mod\BlackICE-ExpandedLocal\BiceExpanded EXTRAS\EVE MARKET DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A5CEBF-3436-463A-AF40-5C9AE025C4C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA99F66B-6E46-48B7-90EA-6604D4B9B8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28050" windowHeight="16440" xr2:uid="{2CADE46B-965D-46B4-A051-9382B4AD2DB2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{2CADE46B-965D-46B4-A051-9382B4AD2DB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,20 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>Lurrus</t>
-  </si>
-  <si>
-    <t>Ragavan</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Expressive Iteration</t>
   </si>
   <si>
-    <t>Omnath</t>
-  </si>
-  <si>
     <t>Solitude</t>
   </si>
   <si>
@@ -63,18 +54,6 @@
     <t>Spike Feeder</t>
   </si>
   <si>
-    <t>Tier 0 (Immediate Ban)</t>
-  </si>
-  <si>
-    <t>Tier 1 (Ban Needed)</t>
-  </si>
-  <si>
-    <t>Tier 2 (Ban Watchlist)</t>
-  </si>
-  <si>
-    <t>Tier 3 (Problem Cards)</t>
-  </si>
-  <si>
     <t>Tasha's Hideous Laughter</t>
   </si>
   <si>
@@ -91,6 +70,54 @@
   </si>
   <si>
     <t>Teferi, Time Raveler</t>
+  </si>
+  <si>
+    <t>Lurrus of the Dream-Den</t>
+  </si>
+  <si>
+    <t>Ragavan, Nimble Pilferer</t>
+  </si>
+  <si>
+    <t>Omnath, Locus of Creation</t>
+  </si>
+  <si>
+    <t>Death's Shadow</t>
+  </si>
+  <si>
+    <t>Dryad of the Ilysian Grove</t>
+  </si>
+  <si>
+    <t>Immediate Bans</t>
+  </si>
+  <si>
+    <t>1 Month Bans</t>
+  </si>
+  <si>
+    <t>2 Month Bans</t>
+  </si>
+  <si>
+    <t>3 Month Bans</t>
+  </si>
+  <si>
+    <t>4 Month Bans</t>
+  </si>
+  <si>
+    <t>Lava Dart</t>
+  </si>
+  <si>
+    <t>Steelshaper's Gift</t>
+  </si>
+  <si>
+    <t>Mutagenic Growth</t>
+  </si>
+  <si>
+    <t>Murktide Regent</t>
+  </si>
+  <si>
+    <t>Recross the Paths</t>
+  </si>
+  <si>
+    <t>Urza, Lord High Artificer</t>
   </si>
 </sst>
 </file>
@@ -146,13 +173,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBBAFB16-9BE0-45C0-838F-DD902B60A18E}" name="Table2" displayName="Table2" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7" xr:uid="{8265A6DA-6432-43D9-AB2E-EC515E5632AC}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4831BBDE-E8A4-4665-AF94-0A07CAE35F8E}" name="Tier 3 (Problem Cards)"/>
-    <tableColumn id="2" xr3:uid="{581DF10E-1436-49DE-8BAB-37751935997B}" name="Tier 2 (Ban Watchlist)"/>
-    <tableColumn id="3" xr3:uid="{4107A6A0-A914-462E-B7CE-2F235DBD4F05}" name="Tier 1 (Ban Needed)"/>
-    <tableColumn id="4" xr3:uid="{15787BE7-C810-4EF3-9996-A5736502481B}" name="Tier 0 (Immediate Ban)"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBBAFB16-9BE0-45C0-838F-DD902B60A18E}" name="Table2" displayName="Table2" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{8265A6DA-6432-43D9-AB2E-EC515E5632AC}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{4831BBDE-E8A4-4665-AF94-0A07CAE35F8E}" name="4 Month Bans"/>
+    <tableColumn id="5" xr3:uid="{71B99F7B-B7FB-432D-B57E-C974E622F27B}" name="3 Month Bans"/>
+    <tableColumn id="2" xr3:uid="{581DF10E-1436-49DE-8BAB-37751935997B}" name="2 Month Bans"/>
+    <tableColumn id="3" xr3:uid="{4107A6A0-A914-462E-B7CE-2F235DBD4F05}" name="1 Month Bans"/>
+    <tableColumn id="4" xr3:uid="{15787BE7-C810-4EF3-9996-A5736502481B}" name="Immediate Bans"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -455,92 +483,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C1A6E5-1817-43CD-AAA1-DE2C59A0FDDE}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
       <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>16</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>